<commit_message>
use county trip gen scaling factor to account for lack of constant. The new trip gen falls short of seed targets and are scaled. This doesn't effect grwoth factors but shall produce reasonable trips when we look at FLUAM trip-ends.
</commit_message>
<xml_diff>
--- a/Input/controlTotals/External_Stns_GrowthFactors.xlsx
+++ b/Input/controlTotals/External_Stns_GrowthFactors.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Input\controlTotals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74198551-C18E-45C9-A7C5-F8204679C08C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322E2531-3047-4E4A-931B-CBDF295B9347}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85E8C833-01CA-4206-A220-C0593A88DEA7}"/>
+    <workbookView xWindow="29310" yWindow="1290" windowWidth="20520" windowHeight="10770" activeTab="1" xr2:uid="{85E8C833-01CA-4206-A220-C0593A88DEA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ext_growthrates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="231">
   <si>
     <t>Year 2020</t>
   </si>
@@ -610,13 +611,130 @@
   </si>
   <si>
     <t>FO 6461 1 0000102</t>
+  </si>
+  <si>
+    <t>TAZ</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>I95</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US1</t>
+  </si>
+  <si>
+    <t>SR121</t>
+  </si>
+  <si>
+    <t>US441</t>
+  </si>
+  <si>
+    <t>US129</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>I75</t>
+  </si>
+  <si>
+    <t>SR145</t>
+  </si>
+  <si>
+    <t>SR53</t>
+  </si>
+  <si>
+    <t>US221</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>SR59</t>
+  </si>
+  <si>
+    <t>US319</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>SR65</t>
+  </si>
+  <si>
+    <t>SR267</t>
+  </si>
+  <si>
+    <t>SR269A</t>
+  </si>
+  <si>
+    <t>SR2</t>
+  </si>
+  <si>
+    <t>SR71</t>
+  </si>
+  <si>
+    <t>US231</t>
+  </si>
+  <si>
+    <t>SR77</t>
+  </si>
+  <si>
+    <t>SR79</t>
+  </si>
+  <si>
+    <t>SR185</t>
+  </si>
+  <si>
+    <t>CR181</t>
+  </si>
+  <si>
+    <t>US331/SR85</t>
+  </si>
+  <si>
+    <t>SR189</t>
+  </si>
+  <si>
+    <t>SR87</t>
+  </si>
+  <si>
+    <t>SR89</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>SR97</t>
+  </si>
+  <si>
+    <t>Muscogee</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
+    <t>US90</t>
+  </si>
+  <si>
+    <t>US98</t>
+  </si>
+  <si>
+    <t>SR292</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,16 +742,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -641,15 +814,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="23">
+    <cellStyle name="Comma 2" xfId="4" xr:uid="{DB0CF21B-09E8-4C8B-A052-BD91672542F3}"/>
+    <cellStyle name="Comma 2 2" xfId="16" xr:uid="{C861441D-BD92-47D9-9FEC-76296BFAC76C}"/>
+    <cellStyle name="Comma 2 3" xfId="17" xr:uid="{DEA79E02-605A-426A-98F6-CCF292435F40}"/>
+    <cellStyle name="Comma 3" xfId="14" xr:uid="{E0B1A336-3893-4B8F-A29B-9AD3E97E3C97}"/>
+    <cellStyle name="Comma 4" xfId="18" xr:uid="{1567B7DF-7842-4683-92D3-E1D638E2FE80}"/>
+    <cellStyle name="Comma 5" xfId="11" xr:uid="{FF100D8C-35AC-4FF9-A25C-F24C8E74A183}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{9D758909-638E-4F48-9803-309A6456B311}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{CA452C5C-B495-4274-8117-80C588207202}"/>
+    <cellStyle name="Normal 2 2 2" xfId="12" xr:uid="{24A0FAC3-2A06-45CF-944D-C0361E7BC8F9}"/>
+    <cellStyle name="Normal 2 3" xfId="15" xr:uid="{918AF4F4-3AD7-4222-8B3B-6BE496B44E3D}"/>
+    <cellStyle name="Normal 2 4" xfId="19" xr:uid="{13F9F14E-D5CA-4105-97AD-5C494B509D90}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{D8495F00-E884-4962-8B11-B0AB1EF0E652}"/>
+    <cellStyle name="Normal 3 2" xfId="6" xr:uid="{9D63E5D7-2E64-4313-8784-89589FA581F9}"/>
+    <cellStyle name="Normal 3 2 2" xfId="20" xr:uid="{FD06E507-084A-4B36-8B7B-EB54FE364AD0}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{C13655E5-0CB3-4F22-8225-DDD258F7AAB3}"/>
+    <cellStyle name="Normal 5" xfId="8" xr:uid="{DDE8462E-4FC3-48C9-9A2F-6E7D421191AC}"/>
+    <cellStyle name="Normal 6" xfId="13" xr:uid="{70AB52E5-67CF-4608-96EE-88397B2D991D}"/>
+    <cellStyle name="Normal 6 2" xfId="21" xr:uid="{21A60BAB-2FD6-44DC-AD7E-69F5B63292E2}"/>
+    <cellStyle name="Normal 7" xfId="1" xr:uid="{B7484ABC-0DF4-4D64-AA25-FB1995875E4A}"/>
+    <cellStyle name="Note 2" xfId="9" xr:uid="{018CA7EC-E60E-4064-BED2-AFB95DF80BBA}"/>
+    <cellStyle name="Percent 2" xfId="10" xr:uid="{C207CBC7-3114-48ED-A037-390E13ED4798}"/>
+    <cellStyle name="Style 1" xfId="22" xr:uid="{8F3F68E4-A682-401F-AE47-98D93458E0CF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -963,7 +1209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66C42F-C1E9-44DA-BD5C-27F65473AC78}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1847,4 +2095,1121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2362983-3373-4563-AF7F-76D1384B51AB}">
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2025</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2030</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2035</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2040</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2045</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>6425</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.1003836481175211</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.0810918396360534</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1.0629635474199148</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.0512668250197941</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1.0426944078327998</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.0370637894451717</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1.0273115096639387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>6426</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.1003836481175211</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.0810918396360534</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.0629635474199148</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.0512668250197941</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.0426944078327998</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.0370637894451717</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1.0273115096639387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>6427</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.1003836481175211</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.0810918396360534</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.0629635474199148</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.0512668250197941</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1.0426944078327998</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1.0370637894451717</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1.0273115096639387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>6428</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.1003836481175211</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.0810918396360534</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.0629635474199148</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.0512668250197941</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1.0426944078327998</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1.0370637894451717</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1.0273115096639387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>6429</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6430</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6431</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>6432</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>6433</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>6434</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>6435</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.0411083691134579</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.0356402036583066</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.0291332847778587</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1.0238853503184713</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.020044928287541</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.017448754870405</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1.0126706626706627</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>6436</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>6437</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>6438</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>6439</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>6440</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>6441</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I18" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>6442</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>6443</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>6444</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>6445</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>6446</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1.03444471964883</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1.0386317907444669</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1.0294459511817124</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1.0233345878810689</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1.0200441338727473</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1.0174869298720028</v>
+      </c>
+      <c r="I23" s="6">
+        <v>1.0114989369241671</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>6447</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H24" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I24" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>6448</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>6449</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>6450</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>6451</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I28" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>6452</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>6453</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F30" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I30" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>6454</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G31" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>6455</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F32" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G32" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I32" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>6456</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F33" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H33" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I33" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>6457</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E34" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F34" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I34" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>6458</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I35" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>6459</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F36" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>6460</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H37" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I37" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>6461</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1.069164537799224</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1.0610520035795963</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1.0479805079186582</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1.0377358490566038</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1.0311934510986644</v>
+      </c>
+      <c r="H38" s="6">
+        <v>1.0268237653547254</v>
+      </c>
+      <c r="I38" s="6">
+        <v>1.0183430989583333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>